<commit_message>
Fixes for target values
</commit_message>
<xml_diff>
--- a/data/producao.xlsx
+++ b/data/producao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandolourenco/SynologyDrive/Programacao/Cursor/pdashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066C4B28-97CE-ED49-9A00-E900C9D5F718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733EFA94-3E59-854D-A69D-004F41E89DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModeloA" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
   <si>
     <t>Total</t>
   </si>
@@ -487,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -569,6 +569,39 @@
         <v>9000</v>
       </c>
       <c r="C7">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>10000</v>
+      </c>
+      <c r="C8">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>11000</v>
+      </c>
+      <c r="C9">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>12000</v>
+      </c>
+      <c r="C10">
         <v>11000</v>
       </c>
     </row>
@@ -1117,7 +1150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0E7C46-6A39-8542-AF88-06AE3993CE84}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>